<commit_message>
begin taking out structure for experiment and add parameters to control adaptive compare and type of TPR calculation
</commit_message>
<xml_diff>
--- a/Data/Paper/Ground_truth_data_status.xlsx
+++ b/Data/Paper/Ground_truth_data_status.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F5A3551-37D2-4450-96D4-F4FFAC8FEA7F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D952644-F648-4912-A30C-BD1FC2969639}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1013" yWindow="727" windowWidth="13605" windowHeight="8326" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="353" yWindow="353" windowWidth="21600" windowHeight="11475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="72">
   <si>
     <t>completely analyzed</t>
   </si>
@@ -236,6 +236,12 @@
   </si>
   <si>
     <t>Machine assisted*</t>
+  </si>
+  <si>
+    <t>rw</t>
+  </si>
+  <si>
+    <t>gs</t>
   </si>
 </sst>
 </file>
@@ -556,10 +562,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q30"/>
+  <dimension ref="A1:R30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="R16" sqref="R16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -574,7 +580,7 @@
     <col min="15" max="15" width="9.06640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>65</v>
       </c>
@@ -615,7 +621,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>62</v>
       </c>
@@ -626,7 +632,7 @@
         <v>1452</v>
       </c>
       <c r="D2" s="3">
-        <f>L2/C2*100</f>
+        <f t="shared" ref="D2:D30" si="0">L2/C2*100</f>
         <v>3.0991735537190084</v>
       </c>
       <c r="E2" s="3">
@@ -658,7 +664,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>62</v>
       </c>
@@ -669,7 +675,7 @@
         <v>455</v>
       </c>
       <c r="D3" s="3">
-        <f>L3/C3*100</f>
+        <f t="shared" si="0"/>
         <v>10.109890109890109</v>
       </c>
       <c r="E3" s="3">
@@ -701,7 +707,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>62</v>
       </c>
@@ -712,7 +718,7 @@
         <v>583</v>
       </c>
       <c r="D4" s="3">
-        <f>L4/C4*100</f>
+        <f t="shared" si="0"/>
         <v>12.178387650085764</v>
       </c>
       <c r="E4" s="3">
@@ -747,7 +753,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>62</v>
       </c>
@@ -758,7 +764,7 @@
         <v>289</v>
       </c>
       <c r="D5" s="3">
-        <f>L5/C5*100</f>
+        <f t="shared" si="0"/>
         <v>30.449826989619378</v>
       </c>
       <c r="E5" s="3">
@@ -790,7 +796,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>62</v>
       </c>
@@ -801,7 +807,7 @@
         <v>3764</v>
       </c>
       <c r="D6" s="3">
-        <f>L6/C6*100</f>
+        <f t="shared" si="0"/>
         <v>6.6418703506907537</v>
       </c>
       <c r="E6" s="3">
@@ -836,7 +842,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>62</v>
       </c>
@@ -847,7 +853,7 @@
         <v>3764</v>
       </c>
       <c r="D7" s="3">
-        <f>L7/C7*100</f>
+        <f t="shared" si="0"/>
         <v>1.1689691817215728</v>
       </c>
       <c r="E7" s="3">
@@ -879,7 +885,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>62</v>
       </c>
@@ -890,7 +896,7 @@
         <v>583</v>
       </c>
       <c r="D8" s="3">
-        <f>L8/C8*100</f>
+        <f t="shared" si="0"/>
         <v>10.291595197255575</v>
       </c>
       <c r="E8" s="3">
@@ -922,7 +928,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>62</v>
       </c>
@@ -933,7 +939,7 @@
         <v>391</v>
       </c>
       <c r="D9" s="3">
-        <f>L9/C9*100</f>
+        <f t="shared" si="0"/>
         <v>23.017902813299234</v>
       </c>
       <c r="E9" s="3">
@@ -965,7 +971,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>62</v>
       </c>
@@ -976,7 +982,7 @@
         <v>576</v>
       </c>
       <c r="D10" s="3">
-        <f>L10/C10*100</f>
+        <f t="shared" si="0"/>
         <v>16.145833333333336</v>
       </c>
       <c r="E10" s="3">
@@ -1008,7 +1014,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>62</v>
       </c>
@@ -1019,7 +1025,7 @@
         <v>1383</v>
       </c>
       <c r="D11" s="3">
-        <f>L11/C11*100</f>
+        <f t="shared" si="0"/>
         <v>4.1937816341287055</v>
       </c>
       <c r="E11" s="3">
@@ -1051,7 +1057,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>62</v>
       </c>
@@ -1062,7 +1068,7 @@
         <v>166</v>
       </c>
       <c r="D12" s="3">
-        <f>L12/C12*100</f>
+        <f t="shared" si="0"/>
         <v>44.578313253012048</v>
       </c>
       <c r="E12" s="3">
@@ -1094,7 +1100,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>63</v>
       </c>
@@ -1105,7 +1111,7 @@
         <v>194</v>
       </c>
       <c r="D13" s="3">
-        <f>L13/C13*100</f>
+        <f t="shared" si="0"/>
         <v>53.608247422680414</v>
       </c>
       <c r="E13" s="3">
@@ -1136,7 +1142,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>63</v>
       </c>
@@ -1147,7 +1153,7 @@
         <v>179</v>
       </c>
       <c r="D14" s="3">
-        <f>L14/C14*100</f>
+        <f t="shared" si="0"/>
         <v>100</v>
       </c>
       <c r="E14" s="3">
@@ -1178,7 +1184,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>63</v>
       </c>
@@ -1189,7 +1195,7 @@
         <v>217</v>
       </c>
       <c r="D15" s="3">
-        <f>L15/C15*100</f>
+        <f t="shared" si="0"/>
         <v>100</v>
       </c>
       <c r="E15" s="3">
@@ -1219,8 +1225,15 @@
       <c r="O15" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.45">
+      <c r="Q15" t="s">
+        <v>71</v>
+      </c>
+      <c r="R15" s="3">
+        <f>SUM(E2:E12)</f>
+        <v>50.187500000000007</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>63</v>
       </c>
@@ -1231,7 +1244,7 @@
         <v>304</v>
       </c>
       <c r="D16" s="3">
-        <f>L16/C16*100</f>
+        <f t="shared" si="0"/>
         <v>100</v>
       </c>
       <c r="E16" s="3">
@@ -1260,6 +1273,13 @@
       </c>
       <c r="O16" s="1" t="s">
         <v>23</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>70</v>
+      </c>
+      <c r="R16" s="3">
+        <f>SUM(E13:E24)</f>
+        <v>91.416666666666657</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.45">
@@ -1273,7 +1293,7 @@
         <v>325</v>
       </c>
       <c r="D17" s="3">
-        <f>L17/C17*100</f>
+        <f t="shared" si="0"/>
         <v>53.846153846153847</v>
       </c>
       <c r="E17" s="3">
@@ -1315,7 +1335,7 @@
         <v>62</v>
       </c>
       <c r="D18" s="3">
-        <f>L18/C18*100</f>
+        <f t="shared" si="0"/>
         <v>100</v>
       </c>
       <c r="E18" s="3">
@@ -1357,7 +1377,7 @@
         <v>443</v>
       </c>
       <c r="D19" s="3">
-        <f>L19/C19*100</f>
+        <f t="shared" si="0"/>
         <v>36.117381489841989</v>
       </c>
       <c r="E19" s="3">
@@ -1399,7 +1419,7 @@
         <v>158</v>
       </c>
       <c r="D20" s="3">
-        <f>L20/C20*100</f>
+        <f t="shared" si="0"/>
         <v>100</v>
       </c>
       <c r="E20" s="3">
@@ -1441,7 +1461,7 @@
         <v>58</v>
       </c>
       <c r="D21" s="3">
-        <f>L21/C21*100</f>
+        <f t="shared" si="0"/>
         <v>100</v>
       </c>
       <c r="E21" s="3">
@@ -1483,7 +1503,7 @@
         <v>13</v>
       </c>
       <c r="D22" s="3">
-        <f>L22/C22*100</f>
+        <f t="shared" si="0"/>
         <v>100</v>
       </c>
       <c r="E22" s="3">
@@ -1525,7 +1545,7 @@
         <v>540</v>
       </c>
       <c r="D23" s="3">
-        <f>L23/C23*100</f>
+        <f t="shared" si="0"/>
         <v>21.481481481481481</v>
       </c>
       <c r="E23" s="3">
@@ -1567,7 +1587,7 @@
         <v>86</v>
       </c>
       <c r="D24" s="3">
-        <f>L24/C24*100</f>
+        <f t="shared" si="0"/>
         <v>100</v>
       </c>
       <c r="E24" s="3">
@@ -1609,7 +1629,7 @@
         <v>1452</v>
       </c>
       <c r="D25" s="3">
-        <f>L25/C25*100</f>
+        <f t="shared" si="0"/>
         <v>3.0991735537190084</v>
       </c>
       <c r="H25" t="s">
@@ -1639,7 +1659,7 @@
         <v>455</v>
       </c>
       <c r="D26" s="3">
-        <f>L26/C26*100</f>
+        <f t="shared" si="0"/>
         <v>10.109890109890109</v>
       </c>
       <c r="H26" t="s">
@@ -1669,7 +1689,7 @@
         <v>583</v>
       </c>
       <c r="D27" s="3">
-        <f>L27/C27*100</f>
+        <f t="shared" si="0"/>
         <v>12.178387650085764</v>
       </c>
       <c r="H27" t="s">
@@ -1699,7 +1719,7 @@
         <v>289</v>
       </c>
       <c r="D28" s="3">
-        <f>L28/C28*100</f>
+        <f t="shared" si="0"/>
         <v>30.449826989619378</v>
       </c>
       <c r="H28" t="s">
@@ -1729,7 +1749,7 @@
         <v>3764</v>
       </c>
       <c r="D29" s="3">
-        <f>L29/C29*100</f>
+        <f t="shared" si="0"/>
         <v>6.6418703506907537</v>
       </c>
       <c r="H29" t="s">
@@ -1759,7 +1779,7 @@
         <v>3764</v>
       </c>
       <c r="D30" s="3">
-        <f>L30/C30*100</f>
+        <f t="shared" si="0"/>
         <v>1.1689691817215728</v>
       </c>
       <c r="H30" t="s">

</xml_diff>

<commit_message>
attempt changes that allow for determination of source sound file in situations (large files) when file is split up into piecies
</commit_message>
<xml_diff>
--- a/Data/Paper/Ground_truth_data_status.xlsx
+++ b/Data/Paper/Ground_truth_data_status.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D952644-F648-4912-A30C-BD1FC2969639}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="353" yWindow="353" windowWidth="21600" windowHeight="11475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="360" yWindow="360" windowWidth="21600" windowHeight="11475"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="76">
   <si>
     <t>completely analyzed</t>
   </si>
@@ -242,12 +241,24 @@
   </si>
   <si>
     <t>gs</t>
+  </si>
+  <si>
+    <t>LM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hand (mooring by hand, randomly selected extent) </t>
+  </si>
+  <si>
+    <t>38:122</t>
+  </si>
+  <si>
+    <t>510:628</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -561,26 +572,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R30"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:R32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="R16" sqref="R16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O33" sqref="O33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.3984375" customWidth="1"/>
-    <col min="4" max="4" width="9.46484375" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.19921875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.19921875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.6640625" customWidth="1"/>
-    <col min="15" max="15" width="9.06640625" style="1"/>
+    <col min="2" max="2" width="7.42578125" customWidth="1"/>
+    <col min="4" max="4" width="9.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.7109375" customWidth="1"/>
+    <col min="15" max="15" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>65</v>
       </c>
@@ -621,7 +632,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>62</v>
       </c>
@@ -632,7 +643,7 @@
         <v>1452</v>
       </c>
       <c r="D2" s="3">
-        <f t="shared" ref="D2:D30" si="0">L2/C2*100</f>
+        <f t="shared" ref="D2:D32" si="0">L2/C2*100</f>
         <v>3.0991735537190084</v>
       </c>
       <c r="E2" s="3">
@@ -664,7 +675,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>62</v>
       </c>
@@ -707,7 +718,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>62</v>
       </c>
@@ -753,7 +764,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>62</v>
       </c>
@@ -796,7 +807,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>62</v>
       </c>
@@ -842,7 +853,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>62</v>
       </c>
@@ -885,7 +896,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>62</v>
       </c>
@@ -928,7 +939,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>62</v>
       </c>
@@ -971,7 +982,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>62</v>
       </c>
@@ -1014,7 +1025,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>62</v>
       </c>
@@ -1057,7 +1068,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>62</v>
       </c>
@@ -1100,7 +1111,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>63</v>
       </c>
@@ -1142,7 +1153,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>63</v>
       </c>
@@ -1184,7 +1195,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>63</v>
       </c>
@@ -1233,7 +1244,7 @@
         <v>50.187500000000007</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>63</v>
       </c>
@@ -1282,7 +1293,7 @@
         <v>91.416666666666657</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>63</v>
       </c>
@@ -1324,7 +1335,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>63</v>
       </c>
@@ -1366,7 +1377,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>63</v>
       </c>
@@ -1408,7 +1419,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>63</v>
       </c>
@@ -1450,7 +1461,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>63</v>
       </c>
@@ -1492,7 +1503,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>63</v>
       </c>
@@ -1534,7 +1545,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>63</v>
       </c>
@@ -1576,7 +1587,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>63</v>
       </c>
@@ -1618,7 +1629,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>26</v>
       </c>
@@ -1648,7 +1659,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>26</v>
       </c>
@@ -1678,7 +1689,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -1708,7 +1719,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>26</v>
       </c>
@@ -1738,7 +1749,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>26</v>
       </c>
@@ -1768,7 +1779,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>26</v>
       </c>
@@ -1796,6 +1807,92 @@
       </c>
       <c r="O30" s="1" t="s">
         <v>27</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>72</v>
+      </c>
+      <c r="B31" t="s">
+        <v>51</v>
+      </c>
+      <c r="C31">
+        <v>633</v>
+      </c>
+      <c r="D31" s="3">
+        <f t="shared" si="0"/>
+        <v>13.270142180094787</v>
+      </c>
+      <c r="E31" s="3">
+        <f>51000/3600</f>
+        <v>14.166666666666666</v>
+      </c>
+      <c r="F31" s="2">
+        <v>41408</v>
+      </c>
+      <c r="G31" s="2">
+        <v>41409</v>
+      </c>
+      <c r="H31" t="s">
+        <v>12</v>
+      </c>
+      <c r="I31" t="s">
+        <v>73</v>
+      </c>
+      <c r="L31">
+        <v>84</v>
+      </c>
+      <c r="M31" t="s">
+        <v>12</v>
+      </c>
+      <c r="N31" t="s">
+        <v>38</v>
+      </c>
+      <c r="O31" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>72</v>
+      </c>
+      <c r="B32" t="s">
+        <v>51</v>
+      </c>
+      <c r="C32">
+        <v>633</v>
+      </c>
+      <c r="D32" s="3">
+        <f t="shared" si="0"/>
+        <v>18.641390205371248</v>
+      </c>
+      <c r="E32">
+        <f>71400/3600</f>
+        <v>19.833333333333332</v>
+      </c>
+      <c r="F32" s="2">
+        <v>41456</v>
+      </c>
+      <c r="G32" s="2">
+        <v>41472</v>
+      </c>
+      <c r="H32" t="s">
+        <v>12</v>
+      </c>
+      <c r="I32" t="s">
+        <v>73</v>
+      </c>
+      <c r="L32">
+        <v>118</v>
+      </c>
+      <c r="M32" t="s">
+        <v>12</v>
+      </c>
+      <c r="N32" t="s">
+        <v>38</v>
+      </c>
+      <c r="O32" s="1" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>